<commit_message>
feat: generate basic chart for b1
OCD-3721
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
+++ b/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TYoung\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{406A5161-47AD-4E85-AB2D-67ACCC2F70C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A859E9-1CD4-4DB3-8EF2-0EEDA952CD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="(b)(1)" sheetId="2" r:id="rId1"/>
@@ -10762,8 +10762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A9C08C-5769-44CA-9721-54F6E9237D58}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12078,7 +12078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7628FA0F-2616-4369-B586-D9F4CA859488}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
feat: update some alignment issues in chart
OCD-3721
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
+++ b/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TYoung\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{397275CE-0C95-4471-89ED-49153700A650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1121C8-EA0C-48B1-9912-84309A8718A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="(b)(1)" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12494805972021503"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.8469468697760274"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -1129,7 +1139,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12515574171799596"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.84669247302970962"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -2040,7 +2060,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12494805972021503"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.8469468697760274"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -2951,7 +2981,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12494805972021503"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.8469468697760274"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -3862,7 +3902,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12494805972021503"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.8469468697760274"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -4773,7 +4823,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12494805972021503"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.8469468697760274"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -5684,7 +5744,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12494805972021503"/>
+          <c:y val="0.12075069311153765"/>
+          <c:w val="0.8469468697760274"/>
+          <c:h val="0.65825764101944073"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -10378,13 +10448,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1788795</xdr:colOff>
+      <xdr:colOff>1741169</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
@@ -10930,7 +11000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E501EB-B624-4B25-B3C2-6AD69F7E81CC}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -12338,7 +12408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F218294-113B-457B-9C2E-9B58E970D337}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
feat: remove 'Synthetic Data' label from chart titles
OCD-3721
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
+++ b/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TYoung\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1121C8-EA0C-48B1-9912-84309A8718A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944B9CB8-0579-40D1-A307-FA83311AD8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="(b)(1)" sheetId="1" r:id="rId1"/>
@@ -174,15 +174,6 @@
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
               <a:t>(b)(1) Cures Update Progress</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1097,15 +1088,6 @@
               <a:t>(b)(2) Cures Update Progress</a:t>
             </a:r>
           </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
-            </a:r>
-          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -2018,15 +2000,6 @@
               <a:t>(e)(1) Cures Update Progress</a:t>
             </a:r>
           </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
-            </a:r>
-          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -2939,15 +2912,6 @@
               <a:t>(f)(5) Cures Update Progress</a:t>
             </a:r>
           </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
-            </a:r>
-          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -3860,15 +3824,6 @@
               <a:t>(g)(6) Cures Update Progress</a:t>
             </a:r>
           </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
-            </a:r>
-          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -4781,15 +4736,6 @@
               <a:t>(g)(9) Cures Update Progress</a:t>
             </a:r>
           </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
-            </a:r>
-          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -5700,15 +5646,6 @@
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
               <a:t>(g)(10) Cures Update Progress</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Synthetic Data</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11000,7 +10937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E501EB-B624-4B25-B3C2-6AD69F7E81CC}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -12408,7 +12345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F218294-113B-457B-9C2E-9B58E970D337}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: remove duplicate dates from excel template
OCD-3721
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
+++ b/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TYoung\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944B9CB8-0579-40D1-A307-FA83311AD8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A25803A-4F81-44EC-86A9-961E5024BA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="(b)(1)" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12494805972021503"/>
-          <c:y val="0.12075069311153765"/>
+          <c:y val="0.1164853913414374"/>
           <c:w val="0.8469468697760274"/>
           <c:h val="0.65825764101944073"/>
         </c:manualLayout>
@@ -799,45 +799,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1711,45 +1678,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -2623,45 +2557,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3535,45 +3436,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -4447,45 +4315,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -5359,45 +5194,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -6271,45 +6073,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="697937487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -10937,8 +10706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E501EB-B624-4B25-B3C2-6AD69F7E81CC}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12345,7 +12114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F218294-113B-457B-9C2E-9B58E970D337}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: remove right axis and change scale in template
OCD-3721
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
+++ b/chpl/chpl-resources/src/main/resources/CuresChartsOverTime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TYoung\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A25803A-4F81-44EC-86A9-961E5024BA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3340E1D7-46C6-4334-B3C0-66D394D91031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="(b)(1)" sheetId="1" r:id="rId1"/>
@@ -871,13 +871,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -1750,13 +1751,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -2629,13 +2631,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -3508,13 +3511,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -4387,13 +4391,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -5266,13 +5271,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -6145,13 +6151,14 @@
         <c:axId val="96027647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -10706,7 +10713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E501EB-B624-4B25-B3C2-6AD69F7E81CC}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
@@ -12114,7 +12121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F218294-113B-457B-9C2E-9B58E970D337}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>